<commit_message>
Version 3 en préparation
</commit_message>
<xml_diff>
--- a/docs/Equilibrage-artefacts.xlsx
+++ b/docs/Equilibrage-artefacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\praxis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D536984B-7948-44BD-AF57-032DBDAA0A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5BC1ED-C555-454A-B94E-E4AD3C4FB91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,8 +123,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -327,14 +327,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -399,7 +399,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -443,51 +443,11 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -500,11 +460,29 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -516,12 +494,21 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -538,13 +525,13 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
@@ -574,6 +561,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -581,22 +577,26 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -692,30 +692,30 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -744,7 +744,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6CAAC7C8-8621-4A45-A8FA-2D45E7623407}" name="Tableau1" displayName="Tableau1" ref="A1:E19" totalsRowCount="1" headerRowDxfId="26" totalsRowDxfId="25" headerRowBorderDxfId="23" tableBorderDxfId="24" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6CAAC7C8-8621-4A45-A8FA-2D45E7623407}" name="Tableau1" displayName="Tableau1" ref="A1:E19" totalsRowCount="1" headerRowDxfId="26" totalsRowDxfId="23" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="22">
   <autoFilter ref="A1:E18" xr:uid="{6CAAC7C8-8621-4A45-A8FA-2D45E7623407}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E18">
     <sortCondition ref="B1:B18"/>
@@ -765,17 +765,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{14682B95-9C1E-4B50-A631-FD16189E7AFD}" name="Tableau3" displayName="Tableau3" ref="H1:K6" totalsRowCount="1" headerRowDxfId="12" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{14682B95-9C1E-4B50-A631-FD16189E7AFD}" name="Tableau3" displayName="Tableau3" ref="H1:K6" totalsRowCount="1" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="H1:K5" xr:uid="{14682B95-9C1E-4B50-A631-FD16189E7AFD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B5A245B6-FA32-448B-B9F2-DF8DA33C6BBA}" name="xValeur" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{F90A1062-DE85-4E26-95A6-433C4D79F41D}" name="xNombre" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="7">
+    <tableColumn id="1" xr3:uid="{B5A245B6-FA32-448B-B9F2-DF8DA33C6BBA}" name="xValeur" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{F90A1062-DE85-4E26-95A6-433C4D79F41D}" name="xNombre" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>SUMIF(Tableau1[Valeur],Tableau3[[#This Row],[xValeur]],Tableau1[Nombre])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{339755BA-B904-420E-8D03-0BD2921BD4BD}" name="xCummul" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="6">
+    <tableColumn id="2" xr3:uid="{339755BA-B904-420E-8D03-0BD2921BD4BD}" name="xCummul" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>SUMIF(Tableau1[Valeur],Tableau3[[#This Row],[xValeur]],Tableau1[Cumul])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A3F67A6B-7B59-4AAF-8701-20B6B41639F3}" name="xProba" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="5" dataCellStyle="Pourcentage">
+    <tableColumn id="3" xr3:uid="{A3F67A6B-7B59-4AAF-8701-20B6B41639F3}" name="xProba" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>SUMIF(Tableau1[Valeur],Tableau3[[#This Row],[xValeur]],Tableau1[Proba])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,15 +1115,15 @@
       </c>
       <c r="I2" s="2">
         <f>SUMIF(Tableau1[Valeur],Tableau3[[#This Row],[xValeur]],Tableau1[Nombre])</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1">
         <f>SUMIF(Tableau1[Valeur],Tableau3[[#This Row],[xValeur]],Tableau1[Cumul])</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="K2" s="14">
         <f>SUMIF(Tableau1[Valeur],Tableau3[[#This Row],[xValeur]],Tableau1[Proba])</f>
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1149,15 +1149,15 @@
       </c>
       <c r="I3" s="2">
         <f>SUMIF(Tableau1[Valeur],Tableau3[[#This Row],[xValeur]],Tableau1[Nombre])</f>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1">
         <f>SUMIF(Tableau1[Valeur],Tableau3[[#This Row],[xValeur]],Tableau1[Cumul])</f>
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="K3" s="14">
         <f>SUMIF(Tableau1[Valeur],Tableau3[[#This Row],[xValeur]],Tableau1[Proba])</f>
-        <v>0.22499999999999998</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1165,14 +1165,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>6</v>
       </c>
       <c r="D4" s="1">
         <f>Tableau1[[#This Row],[Valeur]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E4" s="13">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1199,14 +1199,14 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>6</v>
       </c>
       <c r="D5" s="1">
         <f>Tableau1[[#This Row],[Valeur]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E5" s="13">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1255,11 +1255,11 @@
       </c>
       <c r="J6" s="7">
         <f>SUBTOTAL(109,Tableau3[xCummul])</f>
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="K6" s="16">
         <f>SUBTOTAL(109,Tableau3[xProba])</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B19" s="10">
         <f>SUBTOTAL(101,Tableau1[Valeur])</f>
-        <v>5.2941176470588234</v>
+        <v>5.4117647058823533</v>
       </c>
       <c r="C19" s="1">
         <f>SUBTOTAL(109,Tableau1[Nombre])</f>
@@ -1505,7 +1505,7 @@
       </c>
       <c r="D19" s="1">
         <f>SUBTOTAL(109,Tableau1[Cumul])</f>
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="E19" s="11">
         <f>SUBTOTAL(109,Tableau1[Proba])</f>

</xml_diff>